<commit_message>
moved and added code
</commit_message>
<xml_diff>
--- a/JavaScript/Koch Snowflake Performance Testing/data.xlsx
+++ b/JavaScript/Koch Snowflake Performance Testing/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bogda\OneDrive\Documents\GitHub\Code\JavaScript\Koch Snowflake Performance Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092B6C4D-3DAC-4028-B5DA-4D30D5516DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2FEF98-C759-404C-8695-C6CF74AAC3FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20685" yWindow="7785" windowWidth="17655" windowHeight="12810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -237,6 +237,12 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -246,12 +252,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -259,74 +259,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -603,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,38 +616,38 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="17" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="14" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="J3" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="18" t="s">
+      <c r="K3" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="14" t="s">
         <v>19</v>
       </c>
     </row>
@@ -726,19 +658,19 @@
       <c r="B4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
@@ -1146,10 +1078,10 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="16"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="1">
         <v>140</v>
       </c>
@@ -1193,19 +1125,19 @@
       <c r="B18" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
     </row>
     <row r="19" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
@@ -1242,7 +1174,9 @@
       <c r="K19" s="12">
         <v>1</v>
       </c>
-      <c r="L19" s="12"/>
+      <c r="L19" s="12">
+        <v>1</v>
+      </c>
       <c r="M19" s="12"/>
     </row>
     <row r="20" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1280,6 +1214,9 @@
       <c r="K20" s="2">
         <v>4</v>
       </c>
+      <c r="L20" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="21" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
@@ -1316,6 +1253,9 @@
       <c r="K21" s="2">
         <v>17</v>
       </c>
+      <c r="L21" s="2">
+        <v>16</v>
+      </c>
     </row>
     <row r="22" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
@@ -1352,6 +1292,9 @@
       <c r="K22" s="2">
         <v>65</v>
       </c>
+      <c r="L22" s="2">
+        <v>66</v>
+      </c>
     </row>
     <row r="23" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
@@ -1388,6 +1331,9 @@
       <c r="K23" s="2">
         <v>996</v>
       </c>
+      <c r="L23" s="2">
+        <v>1023</v>
+      </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
@@ -1424,6 +1370,9 @@
       <c r="K24" s="2">
         <v>15681</v>
       </c>
+      <c r="L24" s="2">
+        <v>15985</v>
+      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
@@ -1467,7 +1416,7 @@
         <v>976.5625</v>
       </c>
       <c r="G27" s="2">
-        <f t="shared" ref="G27:G32" si="6">(G19*1000000)/B19</f>
+        <f t="shared" ref="G27:G31" si="6">(G19*1000000)/B19</f>
         <v>976.5625</v>
       </c>
       <c r="H27" s="2">
@@ -1745,6 +1694,6 @@
     <mergeCell ref="C4:M4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>